<commit_message>
aula csp e jogos de tabuleiro
</commit_message>
<xml_diff>
--- a/plano-de-aulas.xlsx
+++ b/plano-de-aulas.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Data</t>
   </si>
@@ -99,6 +99,9 @@
     <t>06/09</t>
   </si>
   <si>
+    <t>08/09</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? O que é uma heurística?</t>
   </si>
   <si>
@@ -108,19 +111,16 @@
     <t xml:space="preserve">Implementação dos algoritmos de busca e dos agentes autônomos em Python para resolver alguns problemas clássicos da literatura. </t>
   </si>
   <si>
-    <t>08/09</t>
-  </si>
-  <si>
     <t>13/09</t>
   </si>
   <si>
+    <t>15/09</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como um agente encontra uma sequência de ações? Quais são os algoritmos que podemos utilizar? Em que cenário utilizar qual algoritmo? O que é uma heurística? </t>
   </si>
   <si>
-    <t xml:space="preserve"> Algoritmos de subida da montanha. Função heurística. Comparação entre algoritmos </t>
-  </si>
-  <si>
-    <t>15/09</t>
+    <t>20/09</t>
   </si>
   <si>
     <t xml:space="preserve">Como unir todos os conceitos e ferramentas apresentados para resolver um problema complexo? </t>
@@ -135,12 +135,45 @@
     <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3 e 4 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>20/09</t>
-  </si>
-  <si>
     <t>22/09</t>
   </si>
   <si>
+    <t>27/09</t>
+  </si>
+  <si>
+    <t>29/09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEMANA DE PROVAS</t>
+  </si>
+  <si>
+    <t>04/10</t>
+  </si>
+  <si>
+    <t>06/10</t>
+  </si>
+  <si>
+    <t>FERIADO</t>
+  </si>
+  <si>
+    <t>11/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como desenvolver um agente autônomo capaz de identificar estados que satisfazem determinadas restrições? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraint Satisfaction Problems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementação de um agente autônomo capaz de identificar estados que satisfazem determinadas restrições.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referências: Cap 5 do AIMA e material fornecido pelo professor.</t>
+  </si>
+  <si>
+    <t>13/10</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como desenvolver um agente autônomo para atuar em ambiente competitivo de soma zero e sem variável aleatória? </t>
   </si>
   <si>
@@ -153,25 +186,16 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios e desenvolvimento de projeto. Referências: Cap 6 do AIMA e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>27/09</t>
-  </si>
-  <si>
-    <t>29/09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEMANA DE PROVAS</t>
-  </si>
-  <si>
-    <t>04/10</t>
-  </si>
-  <si>
-    <t>06/10</t>
-  </si>
-  <si>
-    <t>FERIADO</t>
-  </si>
-  <si>
-    <t>11/10</t>
+    <t>18/10</t>
+  </si>
+  <si>
+    <t>20/10</t>
+  </si>
+  <si>
+    <t>25/10</t>
+  </si>
+  <si>
+    <t>26/10</t>
   </si>
   <si>
     <t xml:space="preserve">O que é aprendizagem por reforço? Qual a sua relação com o desenvolvimento de agentes autônomos? </t>
@@ -186,7 +210,7 @@
     <t xml:space="preserve">Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>13/10</t>
+    <t>27/10</t>
   </si>
   <si>
     <t xml:space="preserve"> Onde é possível executar agentes implementados utilizando aprendizagem por reforço? </t>
@@ -201,7 +225,7 @@
     <t xml:space="preserve"> Aula expositiva com resolução de exercícios. Referências: Cap 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>18/10</t>
+    <t>03/11</t>
   </si>
   <si>
     <t xml:space="preserve"> Quais são os limites e detalhes do algoritmo Q-Learning? </t>
@@ -213,22 +237,22 @@
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning.</t>
   </si>
   <si>
-    <t>20/10</t>
+    <t>08/11</t>
   </si>
   <si>
     <t xml:space="preserve">Quais são os limites e detalhes do algoritmo Q-Learning? </t>
   </si>
   <si>
-    <t>25/10</t>
+    <t>10/11</t>
   </si>
   <si>
     <t xml:space="preserve"> Implementação de agentes autônomos usando o algoritmo Q-Learning. </t>
   </si>
   <si>
-    <t>27/10</t>
-  </si>
-  <si>
-    <t>01/11</t>
+    <t>15/11</t>
+  </si>
+  <si>
+    <t>17/11</t>
   </si>
   <si>
     <t xml:space="preserve"> Quais tipos de problemas podem ser resolvidos através do uso de Agentes Autônomos?</t>
@@ -243,25 +267,13 @@
     <t xml:space="preserve"> Desenvolvimento de projeto. Referências: Cap 1, 2, 3, 4, 6 e 21 do AIMA, Cap. 18 do Géron e material fornecido pelo professor.</t>
   </si>
   <si>
-    <t>03/11</t>
-  </si>
-  <si>
-    <t>08/11</t>
-  </si>
-  <si>
-    <t>10/11</t>
-  </si>
-  <si>
-    <t>15/11</t>
-  </si>
-  <si>
-    <t>17/11</t>
-  </si>
-  <si>
     <t>22/11</t>
   </si>
   <si>
     <t>24/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Copa do Mundo - jogo do Brasil</t>
   </si>
   <si>
     <t>29/11</t>
@@ -346,14 +358,14 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -863,7 +875,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="B17" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -892,7 +904,6 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1"/>
     </row>
     <row r="2" ht="42.75">
       <c r="A2" s="2" t="s">
@@ -907,10 +918,9 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2"/>
     </row>
     <row r="3" ht="57">
       <c r="A3" s="2" t="s">
@@ -928,28 +938,26 @@
       <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3"/>
     </row>
     <row r="4" ht="28.5">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4"/>
     </row>
     <row r="5" ht="28.5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -958,16 +966,15 @@
       <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5"/>
     </row>
     <row r="6" ht="57">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -982,10 +989,9 @@
       <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F6"/>
     </row>
     <row r="7" ht="57">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1005,82 +1011,78 @@
       </c>
     </row>
     <row r="8" ht="57">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8"/>
     </row>
     <row r="9" ht="57">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F9"/>
     </row>
     <row r="10" ht="57">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>33</v>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F10"/>
     </row>
     <row r="11" ht="42.75">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" ht="42.75">
+      <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11"/>
-    </row>
-    <row r="12" ht="42.75">
-      <c r="A12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1092,403 +1094,380 @@
       <c r="E12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F12"/>
     </row>
     <row r="13" ht="42.75">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" ht="42.75">
+      <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="B15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="B16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F13"/>
-    </row>
-    <row r="14" ht="42.75">
-      <c r="A14" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14"/>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="A15" s="5" t="s">
+      <c r="C17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" ht="42.75">
+      <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15"/>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" s="5" t="s">
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16"/>
-    </row>
-    <row r="17" ht="14.25">
-      <c r="A17" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="E18" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17"/>
-    </row>
-    <row r="18" ht="42.75">
-      <c r="A18" s="5" t="s">
+    </row>
+    <row r="19" ht="42.75">
+      <c r="A19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F18"/>
-    </row>
-    <row r="19" ht="42.75">
-      <c r="A19" s="5" t="s">
+    </row>
+    <row r="20" ht="28.5">
+      <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" ht="42.75">
+      <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="B21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" ht="42.75">
+      <c r="A22" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="B22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" ht="28.5">
+      <c r="A23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F19"/>
-    </row>
-    <row r="20" ht="28.5">
-      <c r="A20" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="3" t="s">
+    </row>
+    <row r="24" ht="28.5">
+      <c r="A24" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20"/>
-    </row>
-    <row r="21" ht="28.5">
-      <c r="A21" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21"/>
-    </row>
-    <row r="22" ht="28.5">
-      <c r="A22" s="5" t="s">
+      <c r="D24" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22"/>
-    </row>
-    <row r="23" ht="28.5">
-      <c r="A23" s="5" t="s">
+    </row>
+    <row r="25" ht="28.5">
+      <c r="A25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23"/>
-    </row>
-    <row r="24" ht="42.75">
-      <c r="A24" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="3" t="s">
+    </row>
+    <row r="26" ht="28.5">
+      <c r="A26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="E26" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" ht="42.75">
+      <c r="A27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F24"/>
-    </row>
-    <row r="25" ht="42.75">
-      <c r="A25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25"/>
-    </row>
-    <row r="26" ht="42.75">
-      <c r="A26" s="5" t="s">
+      <c r="D27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26"/>
-    </row>
-    <row r="27" ht="42.75">
-      <c r="A27" s="5" t="s">
+      <c r="E27" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27"/>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" s="5" t="s">
+      <c r="B28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" ht="42.75">
+      <c r="A29" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F28"/>
-    </row>
-    <row r="29" ht="42.75">
-      <c r="A29" s="5" t="s">
+      <c r="B29" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>73</v>
+      <c r="C29" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29"/>
+        <v>83</v>
+      </c>
     </row>
     <row r="30" ht="42.75">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="D30" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F30"/>
+        <v>83</v>
+      </c>
     </row>
     <row r="31" ht="42.75">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" ht="42.75">
+      <c r="A32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31"/>
-    </row>
-    <row r="32" ht="42.75">
-      <c r="A32" s="5" t="s">
+      <c r="E32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33"/>
+      <c r="A33" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34"/>
+      <c r="A34" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="35" ht="14.25"/>
     <row r="36" ht="14.25"/>
@@ -1498,7 +1477,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>